<commit_message>
Add the 8th function.
</commit_message>
<xml_diff>
--- a/results/Taylor_fullsample_0709.xlsx
+++ b/results/Taylor_fullsample_0709.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="25">
   <si>
     <t>Estimator</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>poly_func</t>
+  </si>
+  <si>
+    <t>linear_func</t>
   </si>
   <si>
     <t>co1</t>
@@ -443,7 +446,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P31"/>
+  <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -532,7 +535,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4">
         <v>-0.7098307788537813</v>
@@ -568,7 +571,7 @@
     <row r="5" spans="1:16">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5">
         <v>-0.7562213854315775</v>
@@ -604,7 +607,7 @@
     <row r="6" spans="1:16">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6">
         <v>-0.7154376710589617</v>
@@ -640,7 +643,7 @@
     <row r="7" spans="1:16">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7">
         <v>-0.76168473109413</v>
@@ -678,7 +681,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8">
         <v>-0.7098423444208574</v>
@@ -714,7 +717,7 @@
     <row r="9" spans="1:16">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9">
         <v>-0.7562056532159974</v>
@@ -750,7 +753,7 @@
     <row r="10" spans="1:16">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10">
         <v>-0.6784649633128041</v>
@@ -786,7 +789,7 @@
     <row r="11" spans="1:16">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C11">
         <v>-0.5741324832822018</v>
@@ -824,7 +827,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12">
         <v>-0.7090778190427471</v>
@@ -866,7 +869,7 @@
     <row r="13" spans="1:16">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13">
         <v>-0.7514898821498505</v>
@@ -908,7 +911,7 @@
     <row r="14" spans="1:16">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14">
         <v>-0.9999940587976869</v>
@@ -950,7 +953,7 @@
     <row r="15" spans="1:16">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C15">
         <v>0.4770004025567454</v>
@@ -994,7 +997,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C16">
         <v>-0.7090838634567693</v>
@@ -1036,7 +1039,7 @@
     <row r="17" spans="1:16">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C17">
         <v>-0.7520342927701728</v>
@@ -1078,7 +1081,7 @@
     <row r="18" spans="1:16">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C18">
         <v>-0.7701991830774871</v>
@@ -1120,7 +1123,7 @@
     <row r="19" spans="1:16">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C19">
         <v>-0.5622212636887595</v>
@@ -1164,7 +1167,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C20">
         <v>-0.8170986448583748</v>
@@ -1206,7 +1209,7 @@
     <row r="21" spans="1:16">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C21">
         <v>-0.9844396505278551</v>
@@ -1248,7 +1251,7 @@
     <row r="22" spans="1:16">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C22">
         <v>-0.8559875231972006</v>
@@ -1290,7 +1293,7 @@
     <row r="23" spans="1:16">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C23">
         <v>-0.6703546915091758</v>
@@ -1334,7 +1337,7 @@
         <v>18</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C24">
         <v>-0.7075210742854953</v>
@@ -1376,7 +1379,7 @@
     <row r="25" spans="1:16">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C25">
         <v>-0.7315177951435832</v>
@@ -1418,7 +1421,7 @@
     <row r="26" spans="1:16">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C26">
         <v>-0.04822136368602165</v>
@@ -1460,7 +1463,7 @@
     <row r="27" spans="1:16">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C27">
         <v>-0.6662299390213963</v>
@@ -1504,7 +1507,7 @@
         <v>19</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C28">
         <v>-0.7090694327035109</v>
@@ -1552,7 +1555,7 @@
     <row r="29" spans="1:16">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C29">
         <v>-0.7243892158039617</v>
@@ -1600,7 +1603,7 @@
     <row r="30" spans="1:16">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C30">
         <v>-0.9798197525939597</v>
@@ -1648,7 +1651,7 @@
     <row r="31" spans="1:16">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C31">
         <v>-0.6390860378487534</v>
@@ -1693,8 +1696,178 @@
         <v>-1066.754865483424</v>
       </c>
     </row>
+    <row r="32" spans="1:16">
+      <c r="A32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32">
+        <v>-0.7090672712095367</v>
+      </c>
+      <c r="D32">
+        <v>0.7051408412111475</v>
+      </c>
+      <c r="E32">
+        <v>0.0005270846108141711</v>
+      </c>
+      <c r="F32">
+        <v>-0.07585097507128481</v>
+      </c>
+      <c r="G32">
+        <v>-0.02323376716424582</v>
+      </c>
+      <c r="H32">
+        <v>1.416035604360695</v>
+      </c>
+      <c r="J32">
+        <v>-1.080528565795282</v>
+      </c>
+      <c r="K32">
+        <v>1.074592175897344</v>
+      </c>
+      <c r="L32">
+        <v>0.0005642027868387669</v>
+      </c>
+      <c r="M32">
+        <v>-0.07550442330232486</v>
+      </c>
+      <c r="N32">
+        <v>-0.02307341806374083</v>
+      </c>
+      <c r="O32">
+        <v>0.9289311343387469</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33">
+        <v>-0.7516685886265817</v>
+      </c>
+      <c r="D33">
+        <v>0.6595410402246661</v>
+      </c>
+      <c r="E33">
+        <v>0.06671850804371433</v>
+      </c>
+      <c r="F33">
+        <v>-0.2487130079975295</v>
+      </c>
+      <c r="G33">
+        <v>0.003689032806593822</v>
+      </c>
+      <c r="H33">
+        <v>1.047740175148692</v>
+      </c>
+      <c r="J33">
+        <v>-0.8574933893933496</v>
+      </c>
+      <c r="K33">
+        <v>0.7524733899579436</v>
+      </c>
+      <c r="L33">
+        <v>0.06674306684259475</v>
+      </c>
+      <c r="M33">
+        <v>-0.2491077528920168</v>
+      </c>
+      <c r="N33">
+        <v>0.003692653977174958</v>
+      </c>
+      <c r="O33">
+        <v>0.919095041468339</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34">
+        <v>-0.9999938087821889</v>
+      </c>
+      <c r="D34">
+        <v>-0.003523743343453054</v>
+      </c>
+      <c r="E34">
+        <v>0.05901272340870947</v>
+      </c>
+      <c r="F34">
+        <v>-0.2239929185852499</v>
+      </c>
+      <c r="G34">
+        <v>-0.08319682079167365</v>
+      </c>
+      <c r="H34">
+        <v>0.02634630246596919</v>
+      </c>
+      <c r="J34">
+        <v>-0.7800501824005512</v>
+      </c>
+      <c r="K34">
+        <v>-0.003461882162105671</v>
+      </c>
+      <c r="L34">
+        <v>0.05901831382857809</v>
+      </c>
+      <c r="M34">
+        <v>-0.2239422745182012</v>
+      </c>
+      <c r="N34">
+        <v>-0.08323356207156772</v>
+      </c>
+      <c r="O34">
+        <v>0.03376579041968644</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35">
+        <v>0.4766520604249416</v>
+      </c>
+      <c r="D35">
+        <v>-0.8790920648163564</v>
+      </c>
+      <c r="E35">
+        <v>0.07648983205004396</v>
+      </c>
+      <c r="F35">
+        <v>-0.09020498935921953</v>
+      </c>
+      <c r="G35">
+        <v>0.02352424865596539</v>
+      </c>
+      <c r="H35">
+        <v>0.5277006196296115</v>
+      </c>
+      <c r="J35">
+        <v>-1.472723895481876</v>
+      </c>
+      <c r="K35">
+        <v>-0.02069103131645775</v>
+      </c>
+      <c r="L35">
+        <v>0.07287479566808779</v>
+      </c>
+      <c r="M35">
+        <v>-0.1111105239325738</v>
+      </c>
+      <c r="N35">
+        <v>0.02486304463173006</v>
+      </c>
+      <c r="O35">
+        <v>0.1137925998256436</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="C1:I1"/>
     <mergeCell ref="J1:P1"/>
     <mergeCell ref="A4:A7"/>
@@ -1704,6 +1877,7 @@
     <mergeCell ref="A20:A23"/>
     <mergeCell ref="A24:A27"/>
     <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>